<commit_message>
GRU performance fixed ~kinda :P
</commit_message>
<xml_diff>
--- a/results/GRU/modeling.xlsx
+++ b/results/GRU/modeling.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1391,6 +1391,346 @@
         <v>0.04359246589206352</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>24</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0001969071360761338</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.295071680202894e-07</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.02085443213582039</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.004968228749930859</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.2349011407684074</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.01640518580824816</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>34</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4.954308708654279e-05</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.027730287589487e-06</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.01676929742097855</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.003693493083119392</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.2419355726006238</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.007279144241870948</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>35</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4.63090461339639e-05</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1.612349719343376e-05</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.005075340159237385</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.003563524456694722</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.244540215561469</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.0698721133214506</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>45</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.081165724733026e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1.368856402116335e-06</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.005473521072417498</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.00330555415712297</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.2389582113883663</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.004937563463144684</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>45</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8.632214722101613e-07</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.213804620863432e-06</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.005315640475600958</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.003446863498538733</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.2488232940825086</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.02959955547877408</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>46</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.047117208703457e-05</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.061045628337706e-05</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.007363975513726473</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.003657443448901176</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.2395274915339935</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.02731770837599144</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>36</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3.35233887351799e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.72935903209589e-06</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.00599592924118042</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.00379849155433476</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.2415428440029574</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.3740611493409658</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>42</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3.278416300792034e-07</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.903801849116737e-08</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.006886400282382965</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.003267077961936593</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.2417079557657851</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.007579290575687332</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>29</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.034125341900445e-07</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3.939985410670502e-08</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.005337257869541645</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.003191662020981312</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.2454559858494016</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.1035385409843182</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>43</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3.139947723386321e-07</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2.519928634017416e-07</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.006793499458581209</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.003268587635830045</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.2410615656093686</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.007396387556035302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
bugfix and some other stuff
</commit_message>
<xml_diff>
--- a/results/GRU/modeling.xlsx
+++ b/results/GRU/modeling.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>nhidden</t>
+          <t>n_hdden</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>activation1</t>
+          <t>activation function</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>l1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>l2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dr</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>window_size</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>l1</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>l2</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>dropout_rate</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -475,7 +475,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -495,21 +495,21 @@
         <v>0.1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02332600019872189</v>
+        <v>0.006890535354614258</v>
       </c>
       <c r="H2" t="n">
-        <v>0.005955076776444912</v>
+        <v>0.005014171358197927</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2350314488321579</v>
+        <v>0.2459791614985709</v>
       </c>
       <c r="J2" t="n">
-        <v>0.05839156613232182</v>
+        <v>0.2865930745858573</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -517,67 +517,67 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>2.066456500093838e-05</v>
+        <v>0.005573204065173997</v>
       </c>
       <c r="E3" t="n">
-        <v>6.242528223994966e-05</v>
+        <v>0.003943788133661376</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03021679073572159</v>
+        <v>0.04093680158257484</v>
       </c>
       <c r="H3" t="n">
-        <v>0.006184185389429331</v>
+        <v>0.01022079866379499</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2342879722277733</v>
+        <v>0.2371044479160759</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01824760961679159</v>
+        <v>0.9226218690962914</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1.557339307578796e-05</v>
+        <v>0.0008340552961263116</v>
       </c>
       <c r="E4" t="n">
-        <v>1.885142399573444e-08</v>
+        <v>9.418467206641638e-07</v>
       </c>
       <c r="F4" t="n">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="G4" t="n">
-        <v>0.007819400168955326</v>
+        <v>0.01840993575751781</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003980506677180529</v>
+        <v>0.005726219154894352</v>
       </c>
       <c r="I4" t="n">
-        <v>0.240100674222428</v>
+        <v>0.2343404717875394</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01311306145839315</v>
+        <v>0.1665817456829724</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -585,33 +585,33 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1.420162792087069e-05</v>
+        <v>7.758887103831642e-08</v>
       </c>
       <c r="E5" t="n">
-        <v>2.654985990344387e-06</v>
+        <v>2.470464482417119e-05</v>
       </c>
       <c r="F5" t="n">
         <v>0.25</v>
       </c>
       <c r="G5" t="n">
-        <v>0.007808756548911333</v>
+        <v>0.01471861451864243</v>
       </c>
       <c r="H5" t="n">
-        <v>0.003961288370192051</v>
+        <v>0.005713224876672029</v>
       </c>
       <c r="I5" t="n">
-        <v>0.24163678345025</v>
+        <v>0.2412853134778294</v>
       </c>
       <c r="J5" t="n">
-        <v>0.07867878992207435</v>
+        <v>0.1447871734262371</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -619,33 +619,33 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>6.970644401571223e-09</v>
+        <v>1.010243233521509e-09</v>
       </c>
       <c r="E6" t="n">
-        <v>0.008783726561353384</v>
+        <v>1.163405432159471e-05</v>
       </c>
       <c r="F6" t="n">
-        <v>0.35</v>
+        <v>0.21</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01111716683954</v>
+        <v>0.02861869148910046</v>
       </c>
       <c r="H6" t="n">
-        <v>0.004330058582127094</v>
+        <v>0.005365128628909588</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2385254716944717</v>
+        <v>0.2364816983163744</v>
       </c>
       <c r="J6" t="n">
-        <v>0.09924096309648711</v>
+        <v>0.3645942517021299</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -656,30 +656,30 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>7.949478896145252e-08</v>
+        <v>2.311514150372067e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>0.006275664958346769</v>
+        <v>2.809892340999667e-05</v>
       </c>
       <c r="F7" t="n">
-        <v>0.12</v>
+        <v>0.39</v>
       </c>
       <c r="G7" t="n">
-        <v>0.008261661976575851</v>
+        <v>0.1976224780082703</v>
       </c>
       <c r="H7" t="n">
-        <v>0.006342060398310423</v>
+        <v>0.1050782427191734</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2402673734100173</v>
+        <v>0.2360158996561559</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5394551764305063</v>
+        <v>0.4604893147795405</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -687,67 +687,67 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>7.657525014248624e-05</v>
+        <v>9.656904838179547e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>7.432717009423673e-05</v>
+        <v>0.0002841321051313142</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01312697026878595</v>
+        <v>0.009973255917429924</v>
       </c>
       <c r="H8" t="n">
-        <v>0.00469975546002388</v>
+        <v>0.00468429084867239</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2382968070391417</v>
+        <v>0.2420613374915848</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2316178411294757</v>
+        <v>0.4147909254421874</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>tanh</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2.947310602271065e-05</v>
+        <v>9.791526458549258e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0001142037094919376</v>
+        <v>0.0002156420278451188</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.007600237149745226</v>
+        <v>0.005854007788002491</v>
       </c>
       <c r="H9" t="n">
-        <v>0.003664179937914014</v>
+        <v>0.004113114904612303</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2443357225515486</v>
+        <v>0.2458329214844105</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2832915223641921</v>
+        <v>0.1600962133101078</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -755,33 +755,33 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.383230050435072e-09</v>
+        <v>6.187870403327761e-07</v>
       </c>
       <c r="E10" t="n">
-        <v>6.066446579126689e-08</v>
+        <v>0.0002175859999800288</v>
       </c>
       <c r="F10" t="n">
-        <v>0.32</v>
+        <v>0.15</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01135811023414135</v>
+        <v>0.01325664669275284</v>
       </c>
       <c r="H10" t="n">
-        <v>0.003933241590857506</v>
+        <v>0.004351640120148659</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2390362482337577</v>
+        <v>0.23921545257471</v>
       </c>
       <c r="J10" t="n">
-        <v>0.04273148940652908</v>
+        <v>0.1402950805160191</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -789,33 +789,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>6.395589929499524e-09</v>
+        <v>0.002751608682041008</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00220782627440328</v>
+        <v>0.0006038749470733419</v>
       </c>
       <c r="F11" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01662814430892467</v>
+        <v>0.03581196069717407</v>
       </c>
       <c r="H11" t="n">
-        <v>0.005817936267703772</v>
+        <v>0.007565418258309364</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2392753839249026</v>
+        <v>0.2330476470280999</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1473467284777644</v>
+        <v>0.3667133303931297</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -823,33 +823,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>0.007361105772912924</v>
+        <v>3.344055446851705e-07</v>
       </c>
       <c r="E12" t="n">
-        <v>7.160088586679998e-09</v>
+        <v>2.365884351283e-07</v>
       </c>
       <c r="F12" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.009863745421171188</v>
+        <v>0.003650595434010029</v>
       </c>
       <c r="H12" t="n">
-        <v>0.005103126633912325</v>
+        <v>0.003365897107869387</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2391920034780316</v>
+        <v>0.2458554862007919</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1531391901798116</v>
+        <v>0.1160754073960367</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -857,33 +857,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>9.758788808857499e-07</v>
+        <v>3.802732865687671e-07</v>
       </c>
       <c r="E13" t="n">
-        <v>5.787368515789038e-07</v>
+        <v>2.914652946004195e-07</v>
       </c>
       <c r="F13" t="n">
-        <v>0.49</v>
+        <v>0.01</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02749152109026909</v>
+        <v>0.008978902362287045</v>
       </c>
       <c r="H13" t="n">
-        <v>0.006023879162967205</v>
+        <v>0.003759372048079967</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2335082824205919</v>
+        <v>0.2475860607429706</v>
       </c>
       <c r="J13" t="n">
-        <v>0.02349990006060137</v>
+        <v>0.4672523433647145</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -891,33 +891,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0004570585277007034</v>
+        <v>2.132146673870583e-07</v>
       </c>
       <c r="E14" t="n">
-        <v>5.445538132586004e-05</v>
+        <v>4.967915924468299e-08</v>
       </c>
       <c r="F14" t="n">
-        <v>0.49</v>
+        <v>0.16</v>
       </c>
       <c r="G14" t="n">
-        <v>0.04748203232884407</v>
+        <v>0.005927603226155043</v>
       </c>
       <c r="H14" t="n">
-        <v>0.008375143632292747</v>
+        <v>0.003446208545938134</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2251896235483952</v>
+        <v>0.2464541567826636</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01790340338229214</v>
+        <v>0.05929788781424563</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -928,64 +928,64 @@
         <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001443388776541564</v>
+        <v>2.209899664121555e-08</v>
       </c>
       <c r="E15" t="n">
-        <v>1.52006015446054e-07</v>
+        <v>4.072767162401342e-08</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.04532206058502197</v>
+        <v>0.003707230789586902</v>
       </c>
       <c r="H15" t="n">
-        <v>0.007974543608725071</v>
+        <v>0.005341065116226673</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2261601610525726</v>
+        <v>0.2464577500489501</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01651852674768438</v>
+        <v>4.355845713847558</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00280954159558299</v>
+        <v>2.26136987665149e-08</v>
       </c>
       <c r="E16" t="n">
-        <v>7.59784044936132e-08</v>
+        <v>1.533350843409064e-08</v>
       </c>
       <c r="F16" t="n">
-        <v>0.38</v>
+        <v>0.16</v>
       </c>
       <c r="G16" t="n">
-        <v>0.04280397295951843</v>
+        <v>0.006054870318621397</v>
       </c>
       <c r="H16" t="n">
-        <v>0.007838000543415546</v>
+        <v>0.003812956623733044</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2265044607399169</v>
+        <v>0.240414572886416</v>
       </c>
       <c r="J16" t="n">
-        <v>0.03236408007158564</v>
+        <v>0.1558965095075426</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -996,30 +996,30 @@
         <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>1.218707203925154e-06</v>
+        <v>1.159384389572556e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>9.901231387032703e-08</v>
+        <v>6.283747695317966e-08</v>
       </c>
       <c r="F17" t="n">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0160649549216032</v>
+        <v>0.01363192871212959</v>
       </c>
       <c r="H17" t="n">
-        <v>0.003850617911666632</v>
+        <v>0.003803660860285163</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2367812154873996</v>
+        <v>0.2429476023777372</v>
       </c>
       <c r="J17" t="n">
-        <v>0.06069758947126337</v>
+        <v>0.2979393812629463</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1027,101 +1027,101 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0004721353507941759</v>
+        <v>9.383563265619565e-08</v>
       </c>
       <c r="E18" t="n">
-        <v>7.77162477673193e-09</v>
+        <v>5.114986171114247e-09</v>
       </c>
       <c r="F18" t="n">
-        <v>0.19</v>
+        <v>0.05</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1024162769317627</v>
+        <v>0.004256850574165583</v>
       </c>
       <c r="H18" t="n">
-        <v>0.02187558636069298</v>
+        <v>0.003380968933925033</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2223857227800188</v>
+        <v>0.2465144293957054</v>
       </c>
       <c r="J18" t="n">
-        <v>0.03310917320912661</v>
+        <v>0.1205892487673978</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0004264957665831507</v>
+        <v>9.893668964867965e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>6.329356673255554e-07</v>
+        <v>5.082873956565357e-07</v>
       </c>
       <c r="F19" t="n">
-        <v>0.42</v>
+        <v>0.16</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01187523733824492</v>
+        <v>0.005972257349640131</v>
       </c>
       <c r="H19" t="n">
-        <v>0.004522201139479876</v>
+        <v>0.004052430856972933</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2378927150109155</v>
+        <v>0.2465608062287468</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1291997147108186</v>
+        <v>1.081339605874277</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>3.713308206498919e-06</v>
+        <v>6.02304140114965e-09</v>
       </c>
       <c r="E20" t="n">
-        <v>1.301787628408067e-08</v>
+        <v>3.066836899593702e-06</v>
       </c>
       <c r="F20" t="n">
         <v>0.3</v>
       </c>
       <c r="G20" t="n">
-        <v>0.02493229508399963</v>
+        <v>0.007984091527760029</v>
       </c>
       <c r="H20" t="n">
-        <v>0.004964846652001143</v>
+        <v>0.003892786568030715</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2405089518378668</v>
+        <v>0.2445040773023905</v>
       </c>
       <c r="J20" t="n">
-        <v>0.3638514142095281</v>
+        <v>0.416176689960325</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1129,237 +1129,237 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>1.776368369253149e-07</v>
+        <v>1.727734955475406e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>1.074434315584648e-09</v>
+        <v>3.102473258279525e-09</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0935879647731781</v>
+        <v>0.005747072398662567</v>
       </c>
       <c r="H21" t="n">
-        <v>0.00500305462628603</v>
+        <v>0.003371285507455468</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2295221287338262</v>
+        <v>0.2461777492140539</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2747793462794741</v>
+        <v>0.1005726223013292</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>3</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0001353120031874206</v>
+        <v>3.084321219343157e-06</v>
       </c>
       <c r="E22" t="n">
-        <v>4.482998936584352e-07</v>
+        <v>1.399511478928177e-09</v>
       </c>
       <c r="F22" t="n">
         <v>0.23</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01430204790085554</v>
+        <v>0.009768646210432053</v>
       </c>
       <c r="H22" t="n">
-        <v>0.004463081248104572</v>
+        <v>0.003754369216039777</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2346414653063179</v>
+        <v>0.2427620921348912</v>
       </c>
       <c r="J22" t="n">
-        <v>0.00554651896756447</v>
+        <v>0.06499237126274635</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0001370546003211621</v>
+        <v>4.407190536023993e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>5.380018837563966e-07</v>
+        <v>1.026362878738003e-09</v>
       </c>
       <c r="F23" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01486404705792665</v>
+        <v>0.009687871672213078</v>
       </c>
       <c r="H23" t="n">
-        <v>0.004032167140394449</v>
+        <v>0.004078031983226538</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2404005085654544</v>
+        <v>0.2428541197874781</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1278392963484242</v>
+        <v>0.5550003277461432</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>0.001313742711228813</v>
+        <v>0.0001158070990855641</v>
       </c>
       <c r="E24" t="n">
-        <v>3.62676627350091e-06</v>
+        <v>7.090593421427798e-09</v>
       </c>
       <c r="F24" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01057394128292799</v>
+        <v>0.006484532728791237</v>
       </c>
       <c r="H24" t="n">
-        <v>0.00428747246041894</v>
+        <v>0.003864448284730315</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2380136476842538</v>
+        <v>0.2474752961668571</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01823004110703076</v>
+        <v>0.2556346657436043</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
-        <v>9.909262349880458e-05</v>
+        <v>1.821629966170931e-06</v>
       </c>
       <c r="E25" t="n">
-        <v>4.421083160214355e-06</v>
+        <v>3.883021534481469e-09</v>
       </c>
       <c r="F25" t="n">
-        <v>0.29</v>
+        <v>0.19</v>
       </c>
       <c r="G25" t="n">
-        <v>0.03670724853873253</v>
+        <v>0.01045853924006224</v>
       </c>
       <c r="H25" t="n">
-        <v>0.006151610054075718</v>
+        <v>0.003816228359937668</v>
       </c>
       <c r="I25" t="n">
-        <v>0.228231998514151</v>
+        <v>0.2431775673068639</v>
       </c>
       <c r="J25" t="n">
-        <v>0.07749356724708806</v>
+        <v>0.3748511338166627</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C26" t="n">
         <v>4</v>
       </c>
       <c r="D26" t="n">
-        <v>6.99337424881015e-06</v>
+        <v>6.912967754135769e-05</v>
       </c>
       <c r="E26" t="n">
-        <v>2.740305488450498e-08</v>
+        <v>3.118977613040834e-08</v>
       </c>
       <c r="F26" t="n">
-        <v>0.22</v>
+        <v>0.29</v>
       </c>
       <c r="G26" t="n">
-        <v>0.009718392044305801</v>
+        <v>0.01018312387168407</v>
       </c>
       <c r="H26" t="n">
-        <v>0.003718364052474499</v>
+        <v>0.004213623236864805</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2374257136181843</v>
+        <v>0.2417650800027651</v>
       </c>
       <c r="J26" t="n">
-        <v>0.02639518951628246</v>
+        <v>0.1107514152220674</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>0.001831191366171857</v>
+        <v>1.213912598700673e-07</v>
       </c>
       <c r="E27" t="n">
-        <v>1.779099563113751e-07</v>
+        <v>1.105757831422261e-07</v>
       </c>
       <c r="F27" t="n">
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0117938295006752</v>
+        <v>0.0108032189309597</v>
       </c>
       <c r="H27" t="n">
-        <v>0.004549393430352211</v>
+        <v>0.004045489709824324</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2376779767025609</v>
+        <v>0.2450349181858691</v>
       </c>
       <c r="J27" t="n">
-        <v>0.08885597596577864</v>
+        <v>0.452750227680563</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1367,339 +1367,339 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00791943855920132</v>
+        <v>2.799486934299315e-06</v>
       </c>
       <c r="E28" t="n">
-        <v>4.064164447077e-09</v>
+        <v>4.636099946351154e-09</v>
       </c>
       <c r="F28" t="n">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="G28" t="n">
-        <v>0.05622411519289017</v>
+        <v>0.007111464161425829</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01151925045996904</v>
+        <v>0.00387157965451479</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2269850446897697</v>
+        <v>0.2425669796913381</v>
       </c>
       <c r="J28" t="n">
-        <v>0.04359246589206352</v>
+        <v>0.3816936570567516</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0001969071360761338</v>
+        <v>0.0003784135735494504</v>
       </c>
       <c r="E29" t="n">
-        <v>3.295071680202894e-07</v>
+        <v>1.705392151788692e-09</v>
       </c>
       <c r="F29" t="n">
-        <v>0.44</v>
+        <v>0.34</v>
       </c>
       <c r="G29" t="n">
-        <v>0.02085443213582039</v>
+        <v>0.01324828807264566</v>
       </c>
       <c r="H29" t="n">
-        <v>0.004968228749930859</v>
+        <v>0.004154960624873638</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2349011407684074</v>
+        <v>0.244029770982115</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01640518580824816</v>
+        <v>0.09203143427653779</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>4</v>
       </c>
       <c r="D30" t="n">
-        <v>4.954308708654279e-05</v>
+        <v>0.001420208852652234</v>
       </c>
       <c r="E30" t="n">
-        <v>1.027730287589487e-06</v>
+        <v>1.644735809846346e-08</v>
       </c>
       <c r="F30" t="n">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="G30" t="n">
-        <v>0.01676929742097855</v>
+        <v>0.01106518879532814</v>
       </c>
       <c r="H30" t="n">
-        <v>0.003693493083119392</v>
+        <v>0.004679219331592321</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2419355726006238</v>
+        <v>0.2411804905515721</v>
       </c>
       <c r="J30" t="n">
-        <v>0.007279144241870948</v>
+        <v>0.1098155802291555</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>4.63090461339639e-05</v>
+        <v>0.0003561701340838422</v>
       </c>
       <c r="E31" t="n">
-        <v>1.612349719343376e-05</v>
+        <v>1.31588236263877e-09</v>
       </c>
       <c r="F31" t="n">
-        <v>0.08</v>
+        <v>0.45</v>
       </c>
       <c r="G31" t="n">
-        <v>0.005075340159237385</v>
+        <v>0.01817124709486961</v>
       </c>
       <c r="H31" t="n">
-        <v>0.003563524456694722</v>
+        <v>0.005505506414920092</v>
       </c>
       <c r="I31" t="n">
-        <v>0.244540215561469</v>
+        <v>0.2386516569497626</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0698721133214506</v>
+        <v>0.1069682659771503</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>1.081165724733026e-06</v>
+        <v>2.60027565429041e-05</v>
       </c>
       <c r="E32" t="n">
-        <v>1.368856402116335e-06</v>
+        <v>1.470842026061111e-08</v>
       </c>
       <c r="F32" t="n">
-        <v>0.15</v>
+        <v>0.34</v>
       </c>
       <c r="G32" t="n">
-        <v>0.005473521072417498</v>
+        <v>0.01236096490174532</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00330555415712297</v>
+        <v>0.004200709518045187</v>
       </c>
       <c r="I32" t="n">
-        <v>0.2389582113883663</v>
+        <v>0.2454381049426185</v>
       </c>
       <c r="J32" t="n">
-        <v>0.004937563463144684</v>
+        <v>0.1307087219122492</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>4</v>
       </c>
       <c r="D33" t="n">
-        <v>8.632214722101613e-07</v>
+        <v>5.264400269523006e-06</v>
       </c>
       <c r="E33" t="n">
-        <v>1.213804620863432e-06</v>
+        <v>1.900332129077008e-09</v>
       </c>
       <c r="F33" t="n">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
       <c r="G33" t="n">
-        <v>0.005315640475600958</v>
+        <v>0.007785644382238388</v>
       </c>
       <c r="H33" t="n">
-        <v>0.003446863498538733</v>
+        <v>0.004082770086824894</v>
       </c>
       <c r="I33" t="n">
-        <v>0.2488232940825086</v>
+        <v>0.2419806316385492</v>
       </c>
       <c r="J33" t="n">
-        <v>0.02959955547877408</v>
+        <v>0.1870031663219175</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C34" t="n">
         <v>4</v>
       </c>
       <c r="D34" t="n">
-        <v>1.047117208703457e-05</v>
+        <v>2.289362669240054e-07</v>
       </c>
       <c r="E34" t="n">
-        <v>1.061045628337706e-05</v>
+        <v>2.558051654871096e-09</v>
       </c>
       <c r="F34" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="G34" t="n">
-        <v>0.007363975513726473</v>
+        <v>0.01209523901343346</v>
       </c>
       <c r="H34" t="n">
-        <v>0.003657443448901176</v>
+        <v>0.003757987171411514</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2395274915339935</v>
+        <v>0.2443561587274297</v>
       </c>
       <c r="J34" t="n">
-        <v>0.02731770837599144</v>
+        <v>0.4253637559641448</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>4</v>
       </c>
       <c r="D35" t="n">
-        <v>3.35233887351799e-06</v>
+        <v>0.007594265540556751</v>
       </c>
       <c r="E35" t="n">
-        <v>1.72935903209589e-06</v>
+        <v>1.016574917691001e-09</v>
       </c>
       <c r="F35" t="n">
-        <v>0.15</v>
+        <v>0.33</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00599592924118042</v>
+        <v>0.01233247481286526</v>
       </c>
       <c r="H35" t="n">
-        <v>0.00379849155433476</v>
+        <v>0.005083994474261999</v>
       </c>
       <c r="I35" t="n">
-        <v>0.2415428440029574</v>
+        <v>0.2417999048374637</v>
       </c>
       <c r="J35" t="n">
-        <v>0.3740611493409658</v>
+        <v>0.08345073050387358</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C36" t="n">
         <v>4</v>
       </c>
       <c r="D36" t="n">
-        <v>3.278416300792034e-07</v>
+        <v>0.00985892949595228</v>
       </c>
       <c r="E36" t="n">
-        <v>3.903801849116737e-08</v>
+        <v>1.021411584757447e-08</v>
       </c>
       <c r="F36" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="G36" t="n">
-        <v>0.006886400282382965</v>
+        <v>0.01283777691423893</v>
       </c>
       <c r="H36" t="n">
-        <v>0.003267077961936593</v>
+        <v>0.005747370887547731</v>
       </c>
       <c r="I36" t="n">
-        <v>0.2417079557657851</v>
+        <v>0.2408774688921209</v>
       </c>
       <c r="J36" t="n">
-        <v>0.007579290575687332</v>
+        <v>0.09679066168579062</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>tanh</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" t="n">
-        <v>1.034125341900445e-07</v>
+        <v>0.0005077334688305396</v>
       </c>
       <c r="E37" t="n">
-        <v>3.939985410670502e-08</v>
+        <v>1.152407674416007e-09</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1</v>
+        <v>0.32</v>
       </c>
       <c r="G37" t="n">
-        <v>0.005337257869541645</v>
+        <v>0.009918514639139175</v>
       </c>
       <c r="H37" t="n">
-        <v>0.003191662020981312</v>
+        <v>0.004756949841976166</v>
       </c>
       <c r="I37" t="n">
-        <v>0.2454559858494016</v>
+        <v>0.2402317170309804</v>
       </c>
       <c r="J37" t="n">
-        <v>0.1035385409843182</v>
+        <v>0.3298869498908492</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1707,28 +1707,2544 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>3.139947723386321e-07</v>
+        <v>0.00399644257328729</v>
       </c>
       <c r="E38" t="n">
-        <v>2.519928634017416e-07</v>
+        <v>1.651356736297464e-06</v>
       </c>
       <c r="F38" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.02321113646030426</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.0109770130366087</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.2376640235775645</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.1521894717057189</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>13</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>4</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0002464606131153852</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.044969708991583e-07</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.01678873598575592</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.005060743540525436</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.2366113922242436</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.1511523815340843</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>30</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>3</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.001172956359476045</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.17770842863366e-05</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.008943709544837475</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.004427758976817131</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.2431697972114571</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.1561919737004214</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>46</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3.246982424629543e-08</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.004688026771880249</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0104758869856596</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.003946328535676003</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.2449126839966962</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.1742648302005289</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>38</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2.149819385333915e-05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3.545125831931271e-08</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.008487939834594727</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.00388347776606679</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.2434986254847434</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.1947855739706858</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>36</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.005347032826100293</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1.026665485777863e-08</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.01224214024841785</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.00621759332716465</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.2373285948946912</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.5312277235654812</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>33</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>4</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.007522209718193122</v>
+      </c>
+      <c r="E44" t="n">
+        <v>7.211421291834435e-09</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.01210528984665871</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.005510142538696527</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.2385526891747928</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.2085363572088569</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>40</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.00825255906382562</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3.152135790778249e-09</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.01462219003587961</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.00684308772906661</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.2465888218973784</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1.19418154088317</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>26</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>4</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.002558654070371848</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2.132253868294337e-09</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.01457683369517326</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.005202545318752527</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.241813222634065</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.6071495128507739</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>37</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>3</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.001020846070173784</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2.02333615976157e-08</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.01260791253298521</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.005162107292562723</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.238263175889784</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.1465937049172989</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>34</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" t="n">
+        <v>8.427402650498652e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1.08117578973719e-09</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.007944516837596893</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.003971466328948736</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.2410853590572838</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.1196965864866826</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>21</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>4</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.001985419448451882</v>
+      </c>
+      <c r="E49" t="n">
+        <v>8.349149970409432e-09</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.013834941200912</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.005282402504235506</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.2394540906519295</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.5442687323724306</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>30</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>7.987421046463044e-09</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.001933575050461155</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.009731576777994633</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.005619006231427193</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.244353875740942</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.4057246358148417</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>42</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0006290164278770162</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.919945365517361e-08</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.01220538001507521</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.00487490464001894</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.2394234224544966</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.1187251806570009</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>36</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>3</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0001624416822367775</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6.221214515750724e-05</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.01715961471199989</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.004823389928787947</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.2395348522968853</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.1419039282591102</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>25</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.599324186821868e-06</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.086547065508147e-09</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.005182953085750341</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.003472544252872467</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.2440423531648324</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.06619653270011812</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>20</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" t="n">
+        <v>5.367740603643187e-07</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.879979577422116e-09</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.00576054910197854</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.003398116677999496</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.2479381567636865</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.6460847414314602</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>25</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4.95322663675231e-05</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5.712657470491223e-09</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.004281844478100538</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.003584272926673293</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.2471490927222652</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.237087644425399</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>28</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.084296351431098e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.449123589473034e-09</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.004771049600094557</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.003715545171871781</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.2444648572517331</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.3517405383326788</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>23</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.009284677189003606</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.014444982018085e-08</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.008687682449817657</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.005296381190419197</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.2387342912127968</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.1101581894026823</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.989433010973222e-07</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.002651634804615e-07</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.006555915344506502</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.003375449450686574</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.2447836020604441</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.1103343452201565</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>15</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>2</v>
+      </c>
+      <c r="D59" t="n">
+        <v>4.941246874295303e-08</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.955434278512391e-08</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.01988257467746735</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.004643247462809086</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.2381257237885578</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.4555570629695814</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>39</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="n">
+        <v>9.848316132803335e-07</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.78583333076626e-09</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.007761231623589993</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.003737621707841754</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.2438839302639929</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.2638949275697298</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>47</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.003767905715794228</v>
+      </c>
+      <c r="E61" t="n">
+        <v>5.595866029175126e-08</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.006160978693515062</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.005418587476015091</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.2433466410403271</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.4582159838633081</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>28</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.739689035415723e-06</v>
+      </c>
+      <c r="E62" t="n">
+        <v>5.831430051439038e-09</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.00513395294547081</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.003626347985118628</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.2428951882971848</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.1264510516532174</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>25</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" t="n">
+        <v>4.483044495563283e-06</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.088323492358017e-09</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.005614515393972397</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.003454006742686033</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.2430325590630033</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.0971875779328784</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>18</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4.138261027851457e-06</v>
+      </c>
+      <c r="E64" t="n">
+        <v>3.454319013856767e-09</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.004269639030098915</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.003520985832437873</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.2452788545608696</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.08192251074927914</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>17</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.225992010545788e-09</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1.282734265590343e-08</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.005777595099061728</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.00331788626499474</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.2471472010938795</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.09224112246913706</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>17</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>4</v>
+      </c>
+      <c r="D66" t="n">
+        <v>2.183773001199044e-09</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.645403827635499e-08</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.00422190735116601</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.003338935319334269</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.2477366600634694</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.6308576169911815</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>11</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>4</v>
+      </c>
+      <c r="D67" t="n">
+        <v>3.918226681663335e-09</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.753342510097395e-09</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.004753167275339365</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.003362259827554226</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.2468277500103913</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.1410973454038889</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>19</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>4</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2.824103284831421e-06</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.879877908329124e-09</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.003579175798222423</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.004377449862658978</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.2465393339929041</v>
+      </c>
+      <c r="J68" t="n">
+        <v>3.655325035328088</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>1</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.232379039490978e-05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2.400770258389636e-08</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.02843174524605274</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.005342696327716112</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.2355816487656294</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.2350502116262518</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>5</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>4</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.244823089872819e-08</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.117123649168482e-09</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.005448216572403908</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.003361190669238567</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.2467304240690748</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.0729679734383285</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>7</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.247910136569054e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>6.40732969130162e-07</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.008750492706894875</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.003577690804377198</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.2418246802571737</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.07334988183087737</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>6</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" t="n">
+        <v>6.879200461590712e-08</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.38048997971995e-06</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.009584095329046249</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.003777539823204279</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.241701414493679</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.2271216851404609</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>4</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.366941464947668e-07</v>
+      </c>
+      <c r="E73" t="n">
+        <v>6.441119104714652e-07</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.01614484377205372</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.003972713835537434</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.2402302676019067</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.1146426510905568</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>4</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.880503808429122e-08</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.100221178837372e-09</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.010111796669662</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.003524353029206395</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.2438845784386327</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.1207185758732713</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>7</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>4</v>
+      </c>
+      <c r="D75" t="n">
+        <v>3.830111653107438e-07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>5.59405749294915e-06</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.01161837391555309</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.00421604560688138</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.2406816237323704</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.2554460286065156</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>13</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.592540193222297e-08</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.60145400749235e-09</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.004102153703570366</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.003351836930960417</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.2459571032150409</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.1722785879351389</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>5</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>4</v>
+      </c>
+      <c r="D77" t="n">
+        <v>5.53193321869579e-07</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3.356208294124453e-07</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.008516145870089531</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.003463768400251865</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.2447277975313841</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.1116396361574202</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>3</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D78" t="n">
+        <v>4.875386417523122e-05</v>
+      </c>
+      <c r="E78" t="n">
+        <v>1.000967685497959e-09</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.03564299643039703</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.008026803843677044</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.2302699800626078</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.2275841387987756</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>8</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>4</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.311849528873371e-06</v>
+      </c>
+      <c r="E79" t="n">
+        <v>5.283321720383314e-09</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.008794884197413921</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.003533931449055672</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.2438095875820684</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.07461132567857442</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>8</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" t="n">
+        <v>5.715104337017212e-06</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4.642623878545028e-09</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.008148845285177231</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.003774479497224092</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.2468150146257983</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.1785186875642923</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>4</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" t="n">
+        <v>2.841910740380328e-07</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.546052430731479e-09</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.0166347324848175</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.003993967082351446</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.2399873186262735</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.2966883279180703</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>12</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>4</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1.588490907374163e-06</v>
+      </c>
+      <c r="E82" t="n">
+        <v>6.923738266893245e-09</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.007001942954957485</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.003394939471036196</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.2494555742249591</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.5267241125530264</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>22</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>4</v>
+      </c>
+      <c r="D83" t="n">
+        <v>6.980764521894265e-06</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.592173489847563e-09</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.007077911868691444</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.003499287180602551</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.2434026110525827</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.08218665254988786</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>22</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>4</v>
+      </c>
+      <c r="D84" t="n">
+        <v>6.771912873918101e-06</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.457173312048862e-09</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.007163083646446466</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.003533165203407407</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.248392236690633</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.130772271445307</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>15</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1.135959162346652e-08</v>
+      </c>
+      <c r="E85" t="n">
+        <v>4.80349431187474e-09</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.007837661541998386</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.003954814746975899</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.2435330495074743</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.579618344352075</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>9</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>4</v>
+      </c>
+      <c r="D86" t="n">
+        <v>2.205185094602116e-06</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1.465771962436742e-09</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0.01308236178010702</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.004058041609823704</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.2398079484886804</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.1889616997162085</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>24</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>4</v>
+      </c>
+      <c r="D87" t="n">
+        <v>3.493571867257914e-06</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2.823912216359076e-09</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.005205908324569464</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.003510070731863379</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0.2441069578316951</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.1493863625640207</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>5</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>4</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1.872778101395446e-05</v>
+      </c>
+      <c r="E88" t="n">
+        <v>4.617068845953904e-08</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.01556218508630991</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.004585671238601208</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0.2389540141023688</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.1459230462081753</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>19</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1.324702546509477e-07</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.011172065226171e-07</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.004447825718671083</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.0033776112832129</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.2440295602812888</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.07203977925934804</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>19</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>4</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1.600546346120991e-07</v>
+      </c>
+      <c r="E90" t="n">
+        <v>1.69459159043246e-07</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.004443695303052664</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.003390500554814935</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.2441761056947296</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.09122907119320052</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>23</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>4</v>
+      </c>
+      <c r="D91" t="n">
+        <v>3.137776248230774e-08</v>
+      </c>
+      <c r="E91" t="n">
+        <v>5.507719021018698e-07</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0.01135639287531376</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.003785753156989813</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.2443213764779939</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.5245615159727826</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>21</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>3</v>
+      </c>
+      <c r="D92" t="n">
+        <v>9.333132695713434e-07</v>
+      </c>
+      <c r="E92" t="n">
+        <v>3.294283833318003e-07</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.005028377287089825</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.003868380561470985</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0.2425221061249604</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.2862341346800151</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>26</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>4</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1.302653518112181e-06</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1.524322154585965e-07</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.004136856179684401</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.003405296243727207</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.2465632493108775</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.05755921049967217</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>27</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>4</v>
+      </c>
+      <c r="D94" t="n">
+        <v>9.439995589266059e-08</v>
+      </c>
+      <c r="E94" t="n">
+        <v>9.040839611970004e-08</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.00492571946233511</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.003572846297174692</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0.2510560987265206</v>
+      </c>
+      <c r="J94" t="n">
+        <v>2.266854163077232</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>18</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>4</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1.414621834266023e-06</v>
+      </c>
+      <c r="E95" t="n">
+        <v>1.392744464813743e-07</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.004060867708176374</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.003436104627326131</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.2448981847448767</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.2405761451470924</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>14</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>4</v>
+      </c>
+      <c r="D96" t="n">
+        <v>4.446981177692889e-07</v>
+      </c>
+      <c r="E96" t="n">
+        <v>7.962984893997169e-07</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.00482539227232337</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.003355119377374649</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.2458611100927607</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.1279593330053581</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>24</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>4</v>
+      </c>
+      <c r="D97" t="n">
+        <v>7.423569126354176e-06</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2.754799578116451e-06</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.008656851015985012</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.003622318850830197</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.2465706891627071</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.06851544791044195</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>26</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>4</v>
+      </c>
+      <c r="D98" t="n">
+        <v>3.653131436279316e-06</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.6399097358811e-06</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.008316741324961185</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.003456912003457546</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0.2478265842622275</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.05557053542185644</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>26</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" t="n">
+        <v>6.658123881150505e-07</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.336830150070714e-06</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.01065626833587885</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.005207118578255177</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0.2419138648918239</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.1288775708867913</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>24</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>4</v>
+      </c>
+      <c r="D100" t="n">
+        <v>2.190268391147215e-06</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1.289604773149928e-06</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.008619716390967369</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.003478479804471135</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.249595181334937</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.9417578901784895</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>4</v>
+      </c>
+      <c r="D101" t="n">
+        <v>2.643586555712204e-07</v>
+      </c>
+      <c r="E101" t="n">
+        <v>6.172441352807831e-06</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.008347290568053722</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.00418180925771594</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.2407964078970548</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0.08646503695986742</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>8</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>4</v>
+      </c>
+      <c r="D102" t="n">
+        <v>5.661677419857607e-08</v>
+      </c>
+      <c r="E102" t="n">
+        <v>6.398847379267215e-08</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.01681740209460258</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.003601740347221494</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.2419118420072189</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.1706288477427206</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>25</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>4</v>
+      </c>
+      <c r="D103" t="n">
+        <v>3.844389852228992e-06</v>
+      </c>
+      <c r="E103" t="n">
+        <v>2.27651412234622e-06</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.008727036416530609</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.004848451819270849</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0.2353361214913413</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0.1715787363371174</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>27</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>5</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1.172859061609896e-06</v>
+      </c>
+      <c r="E104" t="n">
+        <v>5.286964418698151e-06</v>
+      </c>
+      <c r="F104" t="n">
         <v>0.22</v>
       </c>
-      <c r="G38" t="n">
-        <v>0.006793499458581209</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.003268587635830045</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.2410615656093686</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.007396387556035302</v>
+      <c r="G104" t="n">
+        <v>0.008368171751499176</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.003505265107378364</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0.2444323190353457</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.2063462499626014</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>29</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>5</v>
+      </c>
+      <c r="D105" t="n">
+        <v>9.249519840115023e-06</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1.978394083046066e-05</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.004242568742483854</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.003426710842177272</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0.244971633901196</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.1230008035697624</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>7</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>5</v>
+      </c>
+      <c r="D106" t="n">
+        <v>2.564003656513581e-06</v>
+      </c>
+      <c r="E106" t="n">
+        <v>2.6607899821615e-07</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.1004233211278915</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.009050873108208179</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0.2283272563417164</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.2663320589709083</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>3</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>8</v>
+      </c>
+      <c r="D107" t="n">
+        <v>7.237391557408364e-07</v>
+      </c>
+      <c r="E107" t="n">
+        <v>3.93430658095876e-07</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.05067944154143333</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.009119147434830666</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0.2306372914079794</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.2886356931643639</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>16</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>5</v>
+      </c>
+      <c r="D108" t="n">
+        <v>3.831258151488131e-08</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1.087229898175292e-06</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0.0212359856814146</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.00385295320302248</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0.2414594224011245</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0.2004785308754128</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>24</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>5</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.36049009031116e-05</v>
+      </c>
+      <c r="E109" t="n">
+        <v>2.712404794104206e-06</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.01059774402529001</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.003864460624754429</v>
+      </c>
+      <c r="I109" t="n">
+        <v>0.242124093863456</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0.08990904799619111</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>20</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>5</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1.852167118729989e-07</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1.457766129294352e-07</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.003276975825428963</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.003275941591709852</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0.2484137530766293</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.07657677603061742</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>21</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>5</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1.235942387028616e-07</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1.42363214675015e-07</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.01539912726730108</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.003540977602824569</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0.2457174904702999</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.4505715547714287</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>20</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>6</v>
+      </c>
+      <c r="D112" t="n">
+        <v>7.799379753678848e-08</v>
+      </c>
+      <c r="E112" t="n">
+        <v>4.373292935627626e-07</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.003279876196756959</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.003369793295860291</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0.2480009844087264</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0.122812294231879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>